<commit_message>
Updated requirements: updated requirement details to include patient page layout
</commit_message>
<xml_diff>
--- a/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
+++ b/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="105">
   <si>
     <t>Following links will be displayed</t>
   </si>
@@ -296,10 +296,57 @@
     <t>Patient Page</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Data</t>
+    <t>Patient Chart</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Patient page should be divided in 3 tabs,
+Details,
+Chart,
+Reports</t>
+  </si>
+  <si>
+    <t>Details -&gt; Patient Details Card</t>
+  </si>
+  <si>
+    <t>Details -&gt; Charts</t>
+  </si>
+  <si>
+    <t>An arrow to show all details (patient and medical details captured while admission)</t>
+  </si>
+  <si>
+    <t>This needs to be discussed furher, Initial idea is to show a series of charts based on the vital parameters being monitored. The way the different charts to be displayed needs to finalized</t>
+  </si>
+  <si>
+    <t>there are multiple ways to display the charts here,
+1. show all charts one by one as user scrolls.
+2. show one or 2 charts and give option to show more charts
+3. show only one chart and provide a option to select the parameters</t>
+  </si>
+  <si>
+    <t>By default the chart will show for last 24 hours, the user needs to be provided to select following options,
+1. Last 24 hours
+2. till now
+3. Select date</t>
+  </si>
+  <si>
+    <t>A card with patient name and reason for admission and hospitalization date.</t>
+  </si>
+  <si>
+    <t>Select date will give user an option to select any date between admission date and current date</t>
+  </si>
+  <si>
+    <t>The data format and configuration required for vital parameters is TBD.</t>
+  </si>
+  <si>
+    <t>Connectivity status
+Ward Name
+Bed icon and Bed number</t>
   </si>
 </sst>
 </file>
@@ -331,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,6 +435,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1080,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,29 +1264,103 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added UI Sketches for Mobile App
</commit_message>
<xml_diff>
--- a/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
+++ b/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Server" sheetId="3" r:id="rId3"/>
     <sheet name="Web UI" sheetId="4" r:id="rId4"/>
     <sheet name="Device App" sheetId="5" r:id="rId5"/>
+    <sheet name="App UI" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
   <si>
     <t>Following links will be displayed</t>
   </si>
@@ -296,31 +297,10 @@
     <t>Patient Page</t>
   </si>
   <si>
-    <t>Patient Chart</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
-    <t>Patient page should be divided in 3 tabs,
-Details,
-Chart,
-Reports</t>
-  </si>
-  <si>
-    <t>Details -&gt; Patient Details Card</t>
-  </si>
-  <si>
-    <t>Details -&gt; Charts</t>
-  </si>
-  <si>
     <t>An arrow to show all details (patient and medical details captured while admission)</t>
-  </si>
-  <si>
-    <t>This needs to be discussed furher, Initial idea is to show a series of charts based on the vital parameters being monitored. The way the different charts to be displayed needs to finalized</t>
   </si>
   <si>
     <t>there are multiple ways to display the charts here,
@@ -347,6 +327,49 @@
     <t>Connectivity status
 Ward Name
 Bed icon and Bed number</t>
+  </si>
+  <si>
+    <t>This needs to be discussed further, Initial idea is to show a series of charts based on the vital parameters being monitored. The way the different charts to be displayed needs to finalized</t>
+  </si>
+  <si>
+    <t>Patient Details Card</t>
+  </si>
+  <si>
+    <t>Patient Details card at the header
+Patient page should be divided in 3 tabs,
+Monitor,
+Actions,
+Chart</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>This should be a list of items to be performed. The items listed depends on the sister chart prepared</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>Tab Actions</t>
+  </si>
+  <si>
+    <t>Every Tab will have a floating menu</t>
+  </si>
+  <si>
+    <t>The items are TBD.</t>
+  </si>
+  <si>
+    <t>Action Bar</t>
+  </si>
+  <si>
+    <t>Tab Control</t>
+  </si>
+  <si>
+    <t>Floating Menu</t>
   </si>
 </sst>
 </file>
@@ -455,6 +478,893 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="209550"/>
+          <a:ext cx="4914900" cy="4057650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="219075"/>
+          <a:ext cx="895350" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Back Button</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2124076" y="219075"/>
+          <a:ext cx="895350" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Bed Number</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5191126" y="228600"/>
+          <a:ext cx="895350" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Connectivity Icon</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4248151" y="209550"/>
+          <a:ext cx="895350" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Notifications</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
+            <a:t> Icon</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="800100"/>
+          <a:ext cx="4876800" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="781051"/>
+          <a:ext cx="1371600" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Patient Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4324350" y="809626"/>
+          <a:ext cx="1371600" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Admission Date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="1114425"/>
+          <a:ext cx="4419600" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Reason For Admission</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1409700"/>
+          <a:ext cx="1638300" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Monitor</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2895600" y="1409700"/>
+          <a:ext cx="1638300" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Actions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4514850" y="1419225"/>
+          <a:ext cx="1600200" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Chart</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>169544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Right Arrow 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="1076325"/>
+          <a:ext cx="257175" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Oval 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5467349" y="3676650"/>
+          <a:ext cx="485775" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>79425</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="3781425"/>
+          <a:ext cx="0" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>41325</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="3933825"/>
+          <a:ext cx="0" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1136,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,15 +2174,15 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -1282,17 +2192,17 @@
         <v>88</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1300,30 +2210,30 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1331,39 +2241,77 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="L3:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added requirements individual patient page components.
</commit_message>
<xml_diff>
--- a/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
+++ b/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="DB changes" sheetId="2" r:id="rId2"/>
     <sheet name="Server" sheetId="3" r:id="rId3"/>
-    <sheet name="Web UI" sheetId="4" r:id="rId4"/>
+    <sheet name="Web App" sheetId="8" r:id="rId4"/>
     <sheet name="Device App" sheetId="5" r:id="rId5"/>
     <sheet name="App UI" sheetId="6" r:id="rId6"/>
+    <sheet name="Web App- OLD" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
   <si>
     <t>Following links will be displayed</t>
   </si>
@@ -298,9 +299,6 @@
   </si>
   <si>
     <t>Layout</t>
-  </si>
-  <si>
-    <t>An arrow to show all details (patient and medical details captured while admission)</t>
   </si>
   <si>
     <t>there are multiple ways to display the charts here,
@@ -315,9 +313,6 @@
 3. Select date</t>
   </si>
   <si>
-    <t>A card with patient name and reason for admission and hospitalization date.</t>
-  </si>
-  <si>
     <t>Select date will give user an option to select any date between admission date and current date</t>
   </si>
   <si>
@@ -335,41 +330,170 @@
     <t>Patient Details Card</t>
   </si>
   <si>
-    <t>Patient Details card at the header
-Patient page should be divided in 3 tabs,
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>Tab Actions</t>
+  </si>
+  <si>
+    <t>Every Tab will have a floating menu</t>
+  </si>
+  <si>
+    <t>The items are TBD.</t>
+  </si>
+  <si>
+    <t>Action Bar</t>
+  </si>
+  <si>
+    <t>Tab Control</t>
+  </si>
+  <si>
+    <t>Floating Menu</t>
+  </si>
+  <si>
+    <t>This should be a list of items to be performed. The items listed depends on the chart prepared</t>
+  </si>
+  <si>
+    <t>Intake</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Vital Parameters</t>
+  </si>
+  <si>
+    <t>Medicines</t>
+  </si>
+  <si>
+    <t>Show a list of parameters to be monitored,
+Parameter Name,
+Frequency
+User should have option to remove any parameter from monitoring</t>
+  </si>
+  <si>
+    <t>Show list of medicines prescribed.
+User will have option to add a medicine and specify frequency
+User should have option to stop the medicine</t>
+  </si>
+  <si>
+    <t>Configurations</t>
+  </si>
+  <si>
+    <t>LIST - Display a list of configured parameters</t>
+  </si>
+  <si>
+    <t>For Monitoring frequency, refer to parameter configuration on Device App</t>
+  </si>
+  <si>
+    <t>ADD - Parameter
+Form Fields
+- Parameter Name
+ - Type (Number or Text)
+- Normal Range (optional)
+- Units ( optional if Text)
+- Select from List of values ( if text)  or Free text
+- Default Monitoring Frequency (optional)</t>
+  </si>
+  <si>
+    <t>A simple list of parameters and link to show details.</t>
+  </si>
+  <si>
+    <t>On click navigate to individual lists</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Intake will display a list of intakes scheduled for patient</t>
+  </si>
+  <si>
+    <t>User can select which parameters needs to be monitored.
+The frequency setting should be 
+- Number of days
+- Before Meal
+- After Meal 
+- Hourly, in Minutes,
+- At specific times
+- Monitoring time frame
+         - Start
+        - End
+Before meal and after meal options are optional
+User can specify that parameter needs to be monitored for e.g every hour or every 15 minutes etc. also user can specify the monitoring time frame and specific timings
+User can provide remarks with each parameter, remarks are optional.</t>
+  </si>
+  <si>
+    <t>User can schedule the intake, fields to be captured,
+- Intake
+- Quantity ( can be specified in ml/free text)
+- Frequency
+Frequency setting should be,
+- Number of Days
+- Interval in hours/minutes
+- at specific time</t>
+  </si>
+  <si>
+    <t>No configuration required</t>
+  </si>
+  <si>
+    <t>Output Chart</t>
+  </si>
+  <si>
+    <t>LIST - Display a list of configured outputs</t>
+  </si>
+  <si>
+    <t>ADD - Output,
+- Name
+- Remarks ( free text) or select from option</t>
+  </si>
+  <si>
+    <t>Show the list of output</t>
+  </si>
+  <si>
+    <t>TBD, need to be decided whether option to add output is required or can be directly modified in the database</t>
+  </si>
+  <si>
+    <t>Show 4 boxes with labels,
+Intake
+Output
+Vital Parameters
+Medicines
+Doctor Orders</t>
+  </si>
+  <si>
+    <t>Doctor orders</t>
+  </si>
+  <si>
+    <t>Display a list of orders from the doctor</t>
+  </si>
+  <si>
+    <t>Adding a order is a free text input. This doctor orders either can be added by a doctor or a nurse or a junior doctor on behalf of the incharge doctor. So with free text, there will be a radio button with label Self or Select Doctor. If user selects as Self, the data will be saved by the user which submitted it. if user selects a doctor, a dropdown will be displayed with Doctor in charge as default selected and user can select other doctor as well.</t>
+  </si>
+  <si>
+    <t>Frequency setting should be
+- Before Meal
+- After Meal (Default Selection)
+- Morning, Afternoon or Night ( Some user friendly control is required here)
+- Every hour with specific time frame
+- or at specific timings
+- Quantity( default) one
+- No of Days.
+- If required ( for e.g if there is fever or high blood pressure etc.)
+The medicines can be modified, which means some medicines to be stopped with immediate effect or the frequecy or quantity can be changed
+option while submitting medicine, nead to give option to select self or a doctor as explained in doctor orders.</t>
+  </si>
+  <si>
+    <t>Patient page should be divided in 3 tabs,
 Monitor,
 Actions,
-Chart</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>This should be a list of items to be performed. The items listed depends on the sister chart prepared</t>
-  </si>
-  <si>
-    <t>Chart</t>
-  </si>
-  <si>
-    <t>Tab Actions</t>
-  </si>
-  <si>
-    <t>Every Tab will have a floating menu</t>
-  </si>
-  <si>
-    <t>The items are TBD.</t>
-  </si>
-  <si>
-    <t>Action Bar</t>
-  </si>
-  <si>
-    <t>Tab Control</t>
-  </si>
-  <si>
-    <t>Floating Menu</t>
+Chart,
+Report</t>
   </si>
 </sst>
 </file>
@@ -448,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,6 +585,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1700,10 +1827,600 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="345" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="L3:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,276 +2759,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L3:L21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added requirements for web : patient management
</commit_message>
<xml_diff>
--- a/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
+++ b/technical/requirement/hospital-patient-file/v1.0/patientcare_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
   <si>
     <t>Following links will be displayed</t>
   </si>
@@ -494,6 +494,146 @@
 Actions,
 Chart,
 Report</t>
+  </si>
+  <si>
+    <t>Patient Management</t>
+  </si>
+  <si>
+    <t>Patient List</t>
+  </si>
+  <si>
+    <t>Lists the patients</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>The data is paginated from the server. Page size options should be "10, 50, 100". With 10 as the default page size.</t>
+  </si>
+  <si>
+    <t>When the patient list is loaded when the page is visited, the list should contain only the patients whose status is hospitalized. The list will be sorted on Patient name ascending by default.
+If patient is admitted 3 times, 3 records will be displayed.</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Row Actions menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter box: this will be shown as collapsed by default </t>
+  </si>
+  <si>
+    <t>Filter parameters,
+Basic Search
+Ward,
+Patient Name,
+Mobile number,
+Registration number,
+Bed number,
+Status,
+Advance Search
+Admission Date ( graeater than, equal to or less than or within a range)</t>
+  </si>
+  <si>
+    <t>List Fields</t>
+  </si>
+  <si>
+    <t>Patient Name
+Ward
+Bed no
+Registration number
+Mobile Number
+Emergency Contact Number
+Status
+Dr In charge
+if patient status is hospitalized, a toggle button to be displayed to discharge the patient.</t>
+  </si>
+  <si>
+    <t>Discharge Patient</t>
+  </si>
+  <si>
+    <t>Discharge date and time to be auto populated and user can change it. Only validation here is discharge date to  be greater than hospitalize date and less than or equal to current time.</t>
+  </si>
+  <si>
+    <t>Add Patient Wizard</t>
+  </si>
+  <si>
+    <t>Capture the details of person accompanying, this details are optional and user can opt to skip and move to new screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following fields to be captured
+Patient Details field
+Name
+Mobile Number
+Check if the patient already exists, if exists show the details available.
+User can edit this details, proceed to show the patient details page required for admission.
+This is first page of Add Patient Wizard
+Apart from details, there should be a field Admission date and time. this date will be auto populated with current time and user can change this date and time.
+</t>
+  </si>
+  <si>
+    <t>Capture the details, this details are optional and user can opt to skip and complete the wizard</t>
+  </si>
+  <si>
+    <t>Page to add the patient
+Wizard buttons
+Save &amp; Close
+Save &amp; Next</t>
+  </si>
+  <si>
+    <t>Person Accompanying
+Fileds TBD
+Wizard buttons
+Save &amp; Close
+Save &amp; Next
+Skip</t>
+  </si>
+  <si>
+    <t>Bed and Ward details
+Fields,
+Ward name - Dropdown
+Bed Number - Text input
+Wizard buttons
+Save &amp; Close
+Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tab control with following tabs
+Personal
+Medical
+1. Person accompanying
+2. Reason for admission
+3. Past history
+4. Investigation done ( internal and external)
+5. treatment to be done
+6. </t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Each of following information to be displayed as cards
+1. Personal Details
+2. Person Accompanying</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Each of following information to be displayed as cards
+1. Reason for admission
+2. Past history
+3. Investigation done (internal and external)
+4. treatment to be done
+5. treatment done
+6. Patient file ( medicines, actions etc)</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Show all the patient data and give option to select different part of data and generate report in pdf format</t>
   </si>
 </sst>
 </file>
@@ -1827,18 +1967,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -1880,7 +2019,9 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>126</v>
       </c>
@@ -1889,8 +2030,10 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
+    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
         <v>128</v>
@@ -1899,83 +2042,177 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
+    <row r="7" spans="2:5" ht="285" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -1992,20 +2229,20 @@
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
@@ -2048,6 +2285,42 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2059,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>